<commit_message>
09. Create Global Map
</commit_message>
<xml_diff>
--- a/Sheets/Scripts/Location2.xlsx
+++ b/Sheets/Scripts/Location2.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scripts&gt;Location2" sheetId="1" r:id="Rce551d49baed49bb"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scripts&gt;Location2" sheetId="1" r:id="Rd69d548d7f3c476b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -149,7 +149,7 @@
     <x:t xml:space="preserve">Молодец.</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> Ты прошел мини-игру.</x:t>
+    <x:t xml:space="preserve"> Ты прошел мини игру.</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Вот место, где можно достать меч</x:t>

</xml_diff>